<commit_message>
3.0.10: Implement auto @Serdeable annotation provided.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainSample.xlsx
+++ b/meta/plainApi/BlancoApiPlainSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F64AFF-70D0-8B45-9675-30E890E033E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E617B4-2B9F-424E-85A2-1B9C11C9219C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="1280" windowWidth="29440" windowHeight="21600" tabRatio="860" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="1280" windowWidth="29440" windowHeight="21600" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="242">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2476,6 +2476,15 @@
   </si>
   <si>
     <t>ArrayList</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>io.micronaut.serde.annotation.Serdeable</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JsonAutoDetect
+@Serdeable</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3380,7 +3389,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3632,10 +3641,88 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3647,9 +3734,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3658,12 +3742,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3695,12 +3773,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3710,80 +3782,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3792,10 +3798,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3807,11 +3816,14 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4403,152 +4415,152 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="162"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="175"/>
-      <c r="D6" s="171" t="s">
+      <c r="B6" s="136"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="130" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="171"/>
+      <c r="E6" s="130"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="162" t="s">
+      <c r="A7" s="129" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="171" t="s">
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="130" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="171"/>
+      <c r="E7" s="130"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="162"/>
-      <c r="C8" s="162"/>
-      <c r="D8" s="171" t="s">
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="130" t="s">
         <v>234</v>
       </c>
-      <c r="E8" s="171"/>
+      <c r="E8" s="130"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="162" t="s">
+      <c r="A9" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="162"/>
-      <c r="C9" s="162"/>
-      <c r="D9" s="171" t="s">
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="171"/>
+      <c r="E9" s="130"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="162" t="s">
+      <c r="A11" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="171" t="s">
+      <c r="B11" s="129"/>
+      <c r="C11" s="129"/>
+      <c r="D11" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="171"/>
+      <c r="E11" s="130"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="131" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="151" t="s">
+      <c r="B12" s="131"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="151"/>
+      <c r="E12" s="133"/>
       <c r="F12" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="131" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="150" t="s">
+      <c r="B13" s="131"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="151"/>
+      <c r="E13" s="133"/>
     </row>
     <row r="14" spans="1:6" ht="55" customHeight="1">
-      <c r="A14" s="134" t="s">
+      <c r="A14" s="131" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="172" t="s">
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="134" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="151"/>
+      <c r="E14" s="133"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="131" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="151"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
       <c r="F15" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="131" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="151"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
       <c r="F16" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="152" t="s">
+      <c r="A17" s="173" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="160" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="136"/>
-      <c r="C18" s="137"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="90" t="s">
         <v>137</v>
       </c>
@@ -4568,15 +4580,15 @@
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="147" t="s">
+      <c r="A20" s="170" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="148"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="149"/>
+      <c r="B20" s="171"/>
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="172"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="91" t="s">
@@ -4620,28 +4632,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="146" t="s">
+      <c r="A25" s="169" t="s">
         <v>183</v>
       </c>
-      <c r="B25" s="146"/>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
+      <c r="B25" s="169"/>
+      <c r="C25" s="169"/>
+      <c r="D25" s="169"/>
+      <c r="E25" s="169"/>
+      <c r="F25" s="169"/>
+      <c r="G25" s="169"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="141"/>
-      <c r="D26" s="141"/>
-      <c r="E26" s="141"/>
-      <c r="F26" s="141"/>
-      <c r="G26" s="142"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="165"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="95"/>
@@ -4652,12 +4664,12 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="106"/>
-      <c r="B27" s="157"/>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="157"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="157"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="102"/>
@@ -4668,12 +4680,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="107"/>
-      <c r="B28" s="158"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="J28" s="102"/>
@@ -4684,12 +4696,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="108"/>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="102"/>
@@ -4702,28 +4714,28 @@
       <c r="C30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="95"/>
@@ -4736,14 +4748,14 @@
       <c r="A33" s="106">
         <v>1</v>
       </c>
-      <c r="B33" s="165" t="s">
+      <c r="B33" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="165"/>
-      <c r="F33" s="165"/>
-      <c r="G33" s="165"/>
+      <c r="C33" s="145"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="102"/>
@@ -4754,12 +4766,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="107"/>
-      <c r="B34" s="166"/>
-      <c r="C34" s="166"/>
-      <c r="D34" s="166"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="166"/>
-      <c r="G34" s="166"/>
+      <c r="B34" s="146"/>
+      <c r="C34" s="146"/>
+      <c r="D34" s="146"/>
+      <c r="E34" s="146"/>
+      <c r="F34" s="146"/>
+      <c r="G34" s="146"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="J34" s="102"/>
@@ -4770,12 +4782,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="108"/>
-      <c r="B35" s="167"/>
-      <c r="C35" s="167"/>
-      <c r="D35" s="167"/>
-      <c r="E35" s="167"/>
-      <c r="F35" s="167"/>
-      <c r="G35" s="167"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="102"/>
@@ -4800,28 +4812,28 @@
       <c r="M36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="143" t="s">
+      <c r="A37" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="B37" s="144"/>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
+      <c r="B37" s="167"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="168"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="164" t="s">
+      <c r="B38" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
-      <c r="F38" s="164"/>
-      <c r="G38" s="164"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="144"/>
+      <c r="G38" s="144"/>
       <c r="H38" s="95"/>
       <c r="I38" s="95"/>
       <c r="J38" s="95"/>
@@ -4832,12 +4844,12 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="106"/>
-      <c r="B39" s="157"/>
-      <c r="C39" s="157"/>
-      <c r="D39" s="157"/>
-      <c r="E39" s="157"/>
-      <c r="F39" s="157"/>
-      <c r="G39" s="168"/>
+      <c r="B39" s="148"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="149"/>
       <c r="H39" s="102"/>
       <c r="I39" s="102"/>
       <c r="J39" s="102"/>
@@ -4848,12 +4860,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="107"/>
-      <c r="B40" s="158"/>
-      <c r="C40" s="158"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="169"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="150"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="150"/>
+      <c r="G40" s="151"/>
       <c r="H40" s="102"/>
       <c r="I40" s="102"/>
       <c r="J40" s="102"/>
@@ -4864,12 +4876,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="108"/>
-      <c r="B41" s="159"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="170"/>
+      <c r="B41" s="152"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="152"/>
+      <c r="E41" s="152"/>
+      <c r="F41" s="152"/>
+      <c r="G41" s="153"/>
       <c r="H41" s="102"/>
       <c r="I41" s="102"/>
       <c r="J41" s="102"/>
@@ -4895,15 +4907,15 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="146" t="s">
+      <c r="A43" s="169" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="146"/>
-      <c r="C43" s="146"/>
-      <c r="D43" s="146"/>
-      <c r="E43" s="146"/>
-      <c r="F43" s="146"/>
-      <c r="G43" s="146"/>
+      <c r="B43" s="169"/>
+      <c r="C43" s="169"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="169"/>
+      <c r="F43" s="169"/>
+      <c r="G43" s="169"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="105" t="s">
@@ -5019,221 +5031,299 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="131" t="s">
+      <c r="A50" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="133"/>
-      <c r="C50" s="131" t="s">
+      <c r="B50" s="159"/>
+      <c r="C50" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="132"/>
-      <c r="E50" s="133"/>
+      <c r="D50" s="158"/>
+      <c r="E50" s="159"/>
       <c r="F50" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="138"/>
-      <c r="B51" s="139"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="139"/>
+      <c r="A51" s="154"/>
+      <c r="B51" s="156"/>
+      <c r="C51" s="154"/>
+      <c r="D51" s="155"/>
+      <c r="E51" s="156"/>
       <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="129"/>
-      <c r="B52" s="130"/>
-      <c r="C52" s="129"/>
-      <c r="D52" s="161"/>
-      <c r="E52" s="130"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="139"/>
+      <c r="E52" s="140"/>
       <c r="F52" s="43"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="129"/>
-      <c r="B53" s="130"/>
-      <c r="C53" s="129"/>
-      <c r="D53" s="161"/>
-      <c r="E53" s="130"/>
+      <c r="A53" s="138"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="43"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="129"/>
-      <c r="B54" s="130"/>
-      <c r="C54" s="129"/>
-      <c r="D54" s="161"/>
-      <c r="E54" s="130"/>
+      <c r="A54" s="138"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="139"/>
+      <c r="E54" s="140"/>
       <c r="F54" s="43"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="129"/>
-      <c r="B55" s="130"/>
-      <c r="C55" s="129"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="130"/>
+      <c r="A55" s="138"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="139"/>
+      <c r="E55" s="140"/>
       <c r="F55" s="43"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="129"/>
-      <c r="B56" s="130"/>
-      <c r="C56" s="129"/>
-      <c r="D56" s="161"/>
-      <c r="E56" s="130"/>
+      <c r="A56" s="138"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="139"/>
+      <c r="E56" s="140"/>
       <c r="F56" s="43"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="129"/>
-      <c r="B57" s="130"/>
-      <c r="C57" s="129"/>
-      <c r="D57" s="161"/>
-      <c r="E57" s="130"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="139"/>
+      <c r="E57" s="140"/>
       <c r="F57" s="43"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="129"/>
-      <c r="B58" s="130"/>
-      <c r="C58" s="129"/>
-      <c r="D58" s="161"/>
-      <c r="E58" s="130"/>
+      <c r="A58" s="138"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="139"/>
+      <c r="E58" s="140"/>
       <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="129"/>
-      <c r="B59" s="130"/>
-      <c r="C59" s="129"/>
-      <c r="D59" s="161"/>
-      <c r="E59" s="130"/>
+      <c r="A59" s="138"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="139"/>
+      <c r="E59" s="140"/>
       <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="129"/>
-      <c r="B60" s="130"/>
-      <c r="C60" s="129"/>
-      <c r="D60" s="161"/>
-      <c r="E60" s="130"/>
+      <c r="A60" s="138"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="139"/>
+      <c r="E60" s="140"/>
       <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="129"/>
-      <c r="B61" s="130"/>
-      <c r="C61" s="129"/>
-      <c r="D61" s="161"/>
-      <c r="E61" s="130"/>
+      <c r="A61" s="138"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="140"/>
       <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="129"/>
-      <c r="B62" s="130"/>
-      <c r="C62" s="129"/>
-      <c r="D62" s="161"/>
-      <c r="E62" s="130"/>
+      <c r="A62" s="138"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="140"/>
       <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="129"/>
-      <c r="B63" s="130"/>
-      <c r="C63" s="129"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="130"/>
+      <c r="A63" s="138"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="139"/>
+      <c r="E63" s="140"/>
       <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="129"/>
-      <c r="B64" s="130"/>
-      <c r="C64" s="129"/>
-      <c r="D64" s="161"/>
-      <c r="E64" s="130"/>
+      <c r="A64" s="138"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="138"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="140"/>
       <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="129"/>
-      <c r="B65" s="130"/>
-      <c r="C65" s="129"/>
-      <c r="D65" s="161"/>
-      <c r="E65" s="130"/>
+      <c r="A65" s="138"/>
+      <c r="B65" s="140"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="139"/>
+      <c r="E65" s="140"/>
       <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="129"/>
-      <c r="B66" s="130"/>
-      <c r="C66" s="129"/>
-      <c r="D66" s="161"/>
-      <c r="E66" s="130"/>
+      <c r="A66" s="138"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="138"/>
+      <c r="D66" s="139"/>
+      <c r="E66" s="140"/>
       <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="129"/>
-      <c r="B67" s="130"/>
-      <c r="C67" s="129"/>
-      <c r="D67" s="161"/>
-      <c r="E67" s="130"/>
+      <c r="A67" s="138"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="138"/>
+      <c r="D67" s="139"/>
+      <c r="E67" s="140"/>
       <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="129"/>
-      <c r="B68" s="130"/>
-      <c r="C68" s="129"/>
-      <c r="D68" s="161"/>
-      <c r="E68" s="130"/>
+      <c r="A68" s="138"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="138"/>
+      <c r="D68" s="139"/>
+      <c r="E68" s="140"/>
       <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="129"/>
-      <c r="B69" s="130"/>
-      <c r="C69" s="129"/>
-      <c r="D69" s="161"/>
-      <c r="E69" s="130"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="139"/>
+      <c r="E69" s="140"/>
       <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="129"/>
-      <c r="B70" s="130"/>
-      <c r="C70" s="129"/>
-      <c r="D70" s="161"/>
-      <c r="E70" s="130"/>
+      <c r="A70" s="138"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="138"/>
+      <c r="D70" s="139"/>
+      <c r="E70" s="140"/>
       <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="129"/>
-      <c r="B71" s="130"/>
-      <c r="C71" s="129"/>
-      <c r="D71" s="161"/>
-      <c r="E71" s="130"/>
+      <c r="A71" s="138"/>
+      <c r="B71" s="140"/>
+      <c r="C71" s="138"/>
+      <c r="D71" s="139"/>
+      <c r="E71" s="140"/>
       <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="129"/>
-      <c r="B72" s="130"/>
-      <c r="C72" s="129"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="130"/>
+      <c r="A72" s="138"/>
+      <c r="B72" s="140"/>
+      <c r="C72" s="138"/>
+      <c r="D72" s="139"/>
+      <c r="E72" s="140"/>
       <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="129"/>
-      <c r="B73" s="130"/>
-      <c r="C73" s="129"/>
-      <c r="D73" s="161"/>
-      <c r="E73" s="130"/>
+      <c r="A73" s="138"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="138"/>
+      <c r="D73" s="139"/>
+      <c r="E73" s="140"/>
       <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="129"/>
-      <c r="B74" s="130"/>
-      <c r="C74" s="129"/>
-      <c r="D74" s="161"/>
-      <c r="E74" s="130"/>
+      <c r="A74" s="138"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="138"/>
+      <c r="D74" s="139"/>
+      <c r="E74" s="140"/>
       <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="155"/>
-      <c r="B75" s="156"/>
-      <c r="C75" s="155"/>
-      <c r="D75" s="163"/>
-      <c r="E75" s="156"/>
+      <c r="A75" s="141"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="142"/>
+      <c r="E75" s="143"/>
       <c r="F75" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
@@ -5250,84 +5340,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="2">
@@ -5526,10 +5538,10 @@
         <v>168</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
@@ -5539,20 +5551,20 @@
         <v>171</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="133"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="132" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="133"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -5610,28 +5622,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="165"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -5649,12 +5661,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="148"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -5672,12 +5684,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -5695,12 +5707,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -5720,28 +5732,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="168"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="164"/>
-      <c r="G29" s="164"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="144"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -5761,14 +5773,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -5786,12 +5798,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -5809,12 +5821,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="167"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -5853,28 +5865,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="143" t="s">
+      <c r="A34" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="168"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -5892,12 +5904,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="168"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -5915,12 +5927,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="151"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -5938,12 +5950,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="170"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -6019,16 +6031,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="182" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="181" t="s">
+      <c r="E42" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="181" t="s">
+      <c r="F42" s="180" t="s">
         <v>171</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -6040,13 +6052,13 @@
       <c r="I42" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="181" t="s">
+      <c r="J42" s="180" t="s">
         <v>238</v>
       </c>
-      <c r="K42" s="181" t="s">
+      <c r="K42" s="180" t="s">
         <v>208</v>
       </c>
-      <c r="L42" s="189" t="s">
+      <c r="L42" s="179" t="s">
         <v>225</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -6058,14 +6070,14 @@
       <c r="O42" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="P42" s="179" t="s">
+      <c r="P42" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="179" t="s">
+      <c r="Q42" s="184"/>
+      <c r="R42" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="180"/>
+      <c r="S42" s="184"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -6074,21 +6086,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="177"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="183"/>
+      <c r="A43" s="178"/>
+      <c r="B43" s="178"/>
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="178"/>
+      <c r="N43" s="178"/>
+      <c r="O43" s="177"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -6104,7 +6116,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="177"/>
+      <c r="U43" s="178"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -6748,26 +6760,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A22:G22"/>
@@ -6784,6 +6776,26 @@
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B35:G35"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -6840,8 +6852,8 @@
   </sheetPr>
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -6976,23 +6988,23 @@
         <v>168</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="27" customHeight="1">
       <c r="A14" s="111" t="s">
         <v>171</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="151" t="s">
-        <v>172</v>
-      </c>
-      <c r="D14" s="151"/>
+      <c r="C14" s="190" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="133"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -7018,28 +7030,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -7051,12 +7063,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -7068,12 +7080,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -7085,12 +7097,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -7106,29 +7118,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="164" t="s">
+      <c r="B24" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="164"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -7143,14 +7155,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -7161,13 +7173,17 @@
       <c r="Q25"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="107"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
+      <c r="A26" s="107">
+        <v>2</v>
+      </c>
+      <c r="B26" s="146" t="s">
+        <v>240</v>
+      </c>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -7179,12 +7195,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -7213,29 +7229,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="168"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="164" t="s">
+      <c r="B30" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="164"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -7248,12 +7264,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -7266,12 +7282,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="169"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="151"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -7283,12 +7299,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="170"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -7341,31 +7357,31 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="181" t="s">
+      <c r="E37" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="181" t="s">
+      <c r="F37" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="181" t="s">
+      <c r="G37" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="181" t="s">
+      <c r="H37" s="180" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="181" t="s">
+      <c r="I37" s="180" t="s">
         <v>230</v>
       </c>
       <c r="J37" s="176" t="s">
@@ -7382,23 +7398,23 @@
       <c r="O37" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P37" s="181" t="s">
+      <c r="P37" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="184"/>
-      <c r="B38" s="184"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="184"/>
-      <c r="H38" s="184"/>
-      <c r="I38" s="184"/>
-      <c r="J38" s="183"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="177"/>
       <c r="K38" s="53" t="s">
         <v>123</v>
       </c>
@@ -7414,7 +7430,7 @@
       <c r="O38" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P38" s="184"/>
+      <c r="P38" s="188"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -7912,6 +7928,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="J37:J38"/>
@@ -7928,19 +7957,6 @@
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8150,10 +8166,10 @@
         <v>168</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="1" t="s">
         <v>170</v>
       </c>
@@ -8163,10 +8179,10 @@
         <v>171</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -8192,28 +8208,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -8225,12 +8241,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -8242,12 +8258,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -8259,12 +8275,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -8280,29 +8296,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="143" t="s">
+      <c r="A25" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="168"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="164"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -8317,14 +8333,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="165" t="s">
+      <c r="B27" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -8336,12 +8352,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -8353,12 +8369,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="167"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -8387,29 +8403,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -8422,12 +8438,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="168"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -8440,12 +8456,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="169"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="151"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -8457,12 +8473,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="170"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -8515,31 +8531,31 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="B39" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="181" t="s">
+      <c r="E39" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="181" t="s">
+      <c r="F39" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="181" t="s">
+      <c r="G39" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H39" s="188" t="s">
+      <c r="H39" s="189" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="188" t="s">
+      <c r="I39" s="189" t="s">
         <v>225</v>
       </c>
       <c r="J39" s="176" t="s">
@@ -8556,23 +8572,23 @@
       <c r="O39" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P39" s="181" t="s">
+      <c r="P39" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="184"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="184"/>
-      <c r="H40" s="184"/>
-      <c r="I40" s="184"/>
-      <c r="J40" s="183"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="177"/>
       <c r="K40" s="53" t="s">
         <v>123</v>
       </c>
@@ -8588,7 +8604,7 @@
       <c r="O40" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P40" s="184"/>
+      <c r="P40" s="188"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -9044,19 +9060,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -9073,6 +9076,19 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -9281,10 +9297,10 @@
         <v>168</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
@@ -9294,20 +9310,20 @@
         <v>171</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="133"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="132" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="133"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -9365,28 +9381,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="165"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -9404,12 +9420,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="148"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -9427,12 +9443,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -9450,12 +9466,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -9475,28 +9491,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="168"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="164"/>
-      <c r="G29" s="164"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="144"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -9516,14 +9532,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -9541,12 +9557,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -9564,12 +9580,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="167"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -9608,28 +9624,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="143" t="s">
+      <c r="A34" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="168"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -9647,12 +9663,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="168"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -9670,12 +9686,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="151"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -9693,12 +9709,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="170"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -9774,16 +9790,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="182" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="181" t="s">
+      <c r="E42" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="181" t="s">
+      <c r="F42" s="180" t="s">
         <v>171</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -9795,13 +9811,13 @@
       <c r="I42" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="181" t="s">
+      <c r="J42" s="180" t="s">
         <v>238</v>
       </c>
-      <c r="K42" s="181" t="s">
+      <c r="K42" s="180" t="s">
         <v>208</v>
       </c>
-      <c r="L42" s="189" t="s">
+      <c r="L42" s="179" t="s">
         <v>225</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -9813,14 +9829,14 @@
       <c r="O42" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="P42" s="179" t="s">
+      <c r="P42" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="179" t="s">
+      <c r="Q42" s="184"/>
+      <c r="R42" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="180"/>
+      <c r="S42" s="184"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -9829,21 +9845,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="177"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="183"/>
+      <c r="A43" s="178"/>
+      <c r="B43" s="178"/>
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="178"/>
+      <c r="N43" s="178"/>
+      <c r="O43" s="177"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -9859,7 +9875,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="177"/>
+      <c r="U43" s="178"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -10501,11 +10517,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="U42:U43"/>
     <mergeCell ref="G42:G43"/>
     <mergeCell ref="H42:H43"/>
@@ -10513,30 +10548,11 @@
     <mergeCell ref="J42:J43"/>
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="L42:L43"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="R42:S42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -10729,10 +10745,10 @@
         <v>168</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
@@ -10742,10 +10758,10 @@
         <v>171</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="133"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -10771,28 +10787,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -10804,12 +10820,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -10821,12 +10837,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -10838,12 +10854,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -10859,29 +10875,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="164" t="s">
+      <c r="B24" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="164"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -10896,14 +10912,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -10915,12 +10931,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -10932,12 +10948,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -10966,29 +10982,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="168"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="164" t="s">
+      <c r="B30" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="164"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -11001,12 +11017,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -11019,12 +11035,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="169"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="151"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -11036,12 +11052,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="170"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -11094,31 +11110,31 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="181" t="s">
+      <c r="E37" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="181" t="s">
+      <c r="F37" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="181" t="s">
+      <c r="G37" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="181" t="s">
+      <c r="H37" s="180" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="181" t="s">
+      <c r="I37" s="180" t="s">
         <v>230</v>
       </c>
       <c r="J37" s="176" t="s">
@@ -11135,23 +11151,23 @@
       <c r="O37" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P37" s="181" t="s">
+      <c r="P37" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="184"/>
-      <c r="B38" s="184"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="184"/>
-      <c r="H38" s="184"/>
-      <c r="I38" s="184"/>
-      <c r="J38" s="183"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="177"/>
       <c r="K38" s="53" t="s">
         <v>123</v>
       </c>
@@ -11167,7 +11183,7 @@
       <c r="O38" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P38" s="184"/>
+      <c r="P38" s="188"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -11665,6 +11681,28 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="G37:G38"/>
     <mergeCell ref="H37:H38"/>
@@ -11672,28 +11710,6 @@
     <mergeCell ref="J37:J38"/>
     <mergeCell ref="K37:L37"/>
     <mergeCell ref="M37:N37"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -11741,7 +11757,7 @@
   </sheetPr>
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -11903,10 +11919,10 @@
         <v>168</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="1" t="s">
         <v>170</v>
       </c>
@@ -11916,10 +11932,10 @@
         <v>171</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -11945,28 +11961,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -11978,12 +11994,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -11995,12 +12011,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -12012,12 +12028,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -12033,29 +12049,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="143" t="s">
+      <c r="A25" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="168"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="164"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -12070,14 +12086,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="165" t="s">
+      <c r="B27" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -12089,12 +12105,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -12106,12 +12122,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="167"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -12140,29 +12156,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -12175,12 +12191,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="168"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -12193,12 +12209,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="169"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="151"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -12210,12 +12226,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="170"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -12268,31 +12284,31 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="B39" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="181" t="s">
+      <c r="E39" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="181" t="s">
+      <c r="F39" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="181" t="s">
+      <c r="G39" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H39" s="188" t="s">
+      <c r="H39" s="189" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="188" t="s">
+      <c r="I39" s="189" t="s">
         <v>225</v>
       </c>
       <c r="J39" s="176" t="s">
@@ -12309,23 +12325,23 @@
       <c r="O39" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P39" s="181" t="s">
+      <c r="P39" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="184"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="184"/>
-      <c r="H40" s="184"/>
-      <c r="I40" s="184"/>
-      <c r="J40" s="183"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="177"/>
       <c r="K40" s="53" t="s">
         <v>123</v>
       </c>
@@ -12341,7 +12357,7 @@
       <c r="O40" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P40" s="184"/>
+      <c r="P40" s="188"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -12797,6 +12813,28 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="G39:G40"/>
     <mergeCell ref="H39:H40"/>
@@ -12804,28 +12842,6 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>